<commit_message>
adding changes in index and presupuesto
</commit_message>
<xml_diff>
--- a/presupuesto/presupuesto.xlsx
+++ b/presupuesto/presupuesto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\UTJ\PROBLEMATICA\presupuesto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE20C80-7695-4D90-BAA6-139C72756367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0271673D-ECC9-4F03-AB4A-75766510D0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B61749D1-D6DA-47DB-9DC7-A474F657FF72}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Presupuesto" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Presupuesto!$A$1:$G$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Presupuesto!$A$1:$G$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
   <si>
     <t>DS-K1TA70MI-T</t>
   </si>
@@ -100,12 +100,6 @@
   </si>
   <si>
     <t>SITE</t>
-  </si>
-  <si>
-    <t>EXTRAS</t>
-  </si>
-  <si>
-    <t>GRAN TOTAL</t>
   </si>
   <si>
     <r>
@@ -209,19 +203,10 @@
     <t>MICROSIM30M2M</t>
   </si>
   <si>
-    <t xml:space="preserve">*precios de lista sin descuento </t>
-  </si>
-  <si>
     <t>kit Localizador Vehicular, Incluye ECO4PLUS3GEPCOM + SIM30M2M + VOUCHER1M + EPCOMGPSMENSUAL</t>
   </si>
   <si>
     <t>Plataforma Avanzada para Rastreo GPS, VIDEO Móvil y Telemática Vehicular / Mensualidad (Licencia para 1 localizador GPS) Marca: EPCOM</t>
-  </si>
-  <si>
-    <t>EPCOMGPSMENSUAL</t>
-  </si>
-  <si>
-    <t>ECO4PLUS3GTKIT</t>
   </si>
   <si>
     <t>Rack Abierto de 19" para Montaje en Pared de 16 Unidades.</t>
@@ -296,6 +281,12 @@
   </si>
   <si>
     <t>Costo de instalación y configuración por servicio/componente</t>
+  </si>
+  <si>
+    <t>*precios de lista sin descuento (sujeto a condiciones)</t>
+  </si>
+  <si>
+    <t>ACCESORIOS/COMPLEMENTOS</t>
   </si>
 </sst>
 </file>
@@ -422,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -482,25 +473,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -580,14 +558,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -698,8 +686,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23811" y="1012031"/>
-          <a:ext cx="8334376" cy="74971"/>
+          <a:off x="23811" y="1038127"/>
+          <a:ext cx="8333234" cy="74971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -889,14 +877,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>35719</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>35719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1047750</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>1073811</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>2248</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -947,15 +935,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>130968</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>964406</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>1077925</xdr:rowOff>
+      <xdr:colOff>976313</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>982675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -983,7 +971,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5667374" y="9477375"/>
+          <a:off x="5679281" y="8227219"/>
           <a:ext cx="833438" cy="839800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1007,13 +995,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>261937</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>11906</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>797718</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>875109</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1066,13 +1054,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>23813</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1083469</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>690562</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1125,13 +1113,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>107157</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>881063</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>559592</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1184,13 +1172,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>71438</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>940594</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>939697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1243,13 +1231,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1047751</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>888850</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1302,13 +1290,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>142876</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>11907</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>797720</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>882849</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1361,13 +1349,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>35720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>328409</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1420,14 +1408,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>23814</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>12624</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>619842</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1479,13 +1467,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>10316</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>404813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1538,13 +1526,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>59533</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>59531</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1059657</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>805798</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1599,13 +1587,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>202407</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>869157</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>726280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1658,13 +1646,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>8928</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>345281</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1717,13 +1705,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>107156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>11906</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>383058</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2197,10 +2185,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K82" sqref="K82"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2212,10 +2200,10 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2301,14 +2289,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="4" t="s">
-        <v>23</v>
+      <c r="F7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2320,9 +2307,8 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4" t="s">
-        <v>24</v>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2401,7 +2387,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="12">
@@ -2438,7 +2424,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="12">
@@ -2475,7 +2461,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="12">
@@ -2498,7 +2484,7 @@
         <v>3252.6479999999997</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2512,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="12">
@@ -2534,8 +2520,8 @@
         <f t="shared" ref="J16" si="11">I16*B16</f>
         <v>7653.4184999999998</v>
       </c>
-      <c r="K16" s="46" t="s">
-        <v>63</v>
+      <c r="K16" s="44" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2546,10 +2532,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="12">
@@ -2572,1197 +2558,904 @@
         <v>8937.6</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="20">
-        <f>SUM(G13:G17)</f>
-        <v>3081.35</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="14"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="15"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="22">
-        <f>G18*0.16</f>
-        <v>493.01600000000002</v>
-      </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="15">
-        <f>SUM(J13:J18)</f>
-        <v>61472.932499999995</v>
-      </c>
-      <c r="K19" s="1"/>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="22">
-        <f>G18+G19</f>
-        <v>3574.366</v>
-      </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="15">
-        <f>J19*1.16</f>
-        <v>71308.601699999985</v>
-      </c>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="1"/>
+      <c r="A21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="23">
+        <v>6</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12">
+        <f>H22</f>
+        <v>493.63</v>
+      </c>
+      <c r="G22" s="12">
+        <f>F22*B22</f>
+        <v>493.63</v>
+      </c>
+      <c r="H22" s="13">
+        <v>493.63</v>
+      </c>
+      <c r="I22" s="14">
+        <f>H22*$I$5</f>
+        <v>9847.9184999999998</v>
+      </c>
+      <c r="J22" s="15">
+        <f>I22*B22</f>
+        <v>9847.9184999999998</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="23">
+        <v>7</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12">
+        <f>H23</f>
+        <v>23.63</v>
+      </c>
+      <c r="G23" s="12">
+        <f t="shared" ref="G23" si="12">F23*B23</f>
+        <v>23.63</v>
+      </c>
+      <c r="H23" s="13">
+        <v>23.63</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" ref="I23" si="13">H23*$I$5</f>
+        <v>471.41849999999994</v>
+      </c>
+      <c r="J23" s="15">
+        <f>I23*B23</f>
+        <v>471.41849999999994</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F24" s="29"/>
       <c r="G24" s="30"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23">
+        <v>8</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12">
+        <f>H28</f>
+        <v>229</v>
+      </c>
+      <c r="G28" s="12">
+        <f>F28*B28</f>
+        <v>229</v>
+      </c>
+      <c r="H28" s="13">
+        <v>229</v>
+      </c>
+      <c r="I28" s="14">
+        <f>H28*$I$5</f>
+        <v>4568.55</v>
+      </c>
+      <c r="J28" s="15">
+        <f>I28*B28</f>
+        <v>4568.55</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B29" s="10">
         <v>1</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="12">
         <f>H29</f>
-        <v>493.63</v>
+        <v>4.75</v>
       </c>
       <c r="G29" s="12">
-        <f>F29*B29</f>
-        <v>493.63</v>
+        <f t="shared" ref="G29:G32" si="14">F29*B29</f>
+        <v>4.75</v>
       </c>
       <c r="H29" s="13">
-        <v>493.63</v>
+        <v>4.75</v>
       </c>
       <c r="I29" s="14">
-        <f>H29*$I$5</f>
-        <v>9847.9184999999998</v>
+        <f t="shared" ref="I29:I30" si="15">H29*$I$5</f>
+        <v>94.762500000000003</v>
       </c>
       <c r="J29" s="15">
         <f>I29*B29</f>
-        <v>9847.9184999999998</v>
+        <v>94.762500000000003</v>
       </c>
       <c r="K29" s="24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B30" s="10">
         <v>1</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="12">
         <f>H30</f>
-        <v>23.63</v>
+        <v>5.2</v>
       </c>
       <c r="G30" s="12">
-        <f t="shared" ref="G30" si="12">F30*B30</f>
-        <v>23.63</v>
+        <f t="shared" si="14"/>
+        <v>5.2</v>
       </c>
       <c r="H30" s="13">
-        <v>23.63</v>
+        <v>5.2</v>
       </c>
       <c r="I30" s="14">
-        <f t="shared" ref="I30" si="13">H30*$I$5</f>
-        <v>471.41849999999994</v>
+        <f t="shared" si="15"/>
+        <v>103.74</v>
       </c>
       <c r="J30" s="15">
         <f>I30*B30</f>
-        <v>471.41849999999994</v>
-      </c>
-      <c r="K30" s="31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="20">
-        <f>SUM(G29:G30)</f>
-        <v>517.26</v>
-      </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
+        <v>103.74</v>
+      </c>
+      <c r="K30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
+        <v>11</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="12">
+        <f>H31</f>
+        <v>141.25</v>
+      </c>
+      <c r="G31" s="12">
+        <f>F31*B31</f>
+        <v>141.25</v>
+      </c>
+      <c r="H31" s="13">
+        <v>141.25</v>
+      </c>
+      <c r="I31" s="14">
+        <f t="shared" ref="I31:I32" si="16">H31*$I$5</f>
+        <v>2817.9375</v>
+      </c>
       <c r="J31" s="15">
-        <f>SUM(J29:J30)</f>
-        <v>10319.337</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="22">
-        <f>G31*0.16</f>
-        <v>82.761600000000001</v>
-      </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="15"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="19" t="s">
+        <f t="shared" ref="J31:J32" si="17">I31*B31</f>
+        <v>2817.9375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
         <v>12</v>
       </c>
-      <c r="G33" s="22">
-        <f>G31+G32</f>
-        <v>600.02160000000003</v>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="15">
-        <f>J31*1.16</f>
-        <v>11970.430919999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F34" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12">
+        <f>H32</f>
+        <v>4.5</v>
+      </c>
+      <c r="G32" s="12">
+        <f t="shared" si="14"/>
+        <v>4.5</v>
+      </c>
+      <c r="H32" s="13">
+        <v>4.5</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="16"/>
+        <v>89.774999999999991</v>
+      </c>
+      <c r="J32" s="15">
+        <f t="shared" si="17"/>
+        <v>89.774999999999991</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="45"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="45"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="45"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F37" s="29"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="6"/>
-      <c r="F38" s="7" t="s">
+      <c r="E40" s="6"/>
+      <c r="F40" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
-        <v>8</v>
-      </c>
-      <c r="B39" s="10">
-        <v>1</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12">
-        <f>H54</f>
-        <v>229</v>
-      </c>
-      <c r="G39" s="12">
-        <f>F39*B39</f>
-        <v>229</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23">
-        <v>9</v>
-      </c>
-      <c r="B40" s="10">
-        <v>1</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12">
-        <f>H55</f>
-        <v>4.75</v>
-      </c>
-      <c r="G40" s="12">
-        <f t="shared" ref="G40:G43" si="14">F40*B40</f>
-        <v>4.75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B41" s="10">
         <v>1</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="12">
-        <f>H56</f>
-        <v>5.2</v>
+        <f>H41</f>
+        <v>75</v>
       </c>
       <c r="G41" s="12">
-        <f t="shared" si="14"/>
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f>F41*B41</f>
+        <v>75</v>
+      </c>
+      <c r="H41" s="13">
+        <v>75</v>
+      </c>
+      <c r="I41" s="14">
+        <f>H41*$I$5</f>
+        <v>1496.25</v>
+      </c>
+      <c r="J41" s="15">
+        <f>I41*B41</f>
+        <v>1496.25</v>
+      </c>
+      <c r="K41" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B42" s="10">
         <v>1</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E42" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="E42" s="11"/>
       <c r="F42" s="12">
-        <f>H57</f>
-        <v>141.25</v>
+        <f>H42</f>
+        <v>36.94</v>
       </c>
       <c r="G42" s="12">
-        <f t="shared" si="14"/>
-        <v>141.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G42:G44" si="18">F42*B42</f>
+        <v>36.94</v>
+      </c>
+      <c r="H42" s="13">
+        <v>36.94</v>
+      </c>
+      <c r="I42" s="14">
+        <f t="shared" ref="I42:I44" si="19">H42*$I$5</f>
+        <v>736.95299999999997</v>
+      </c>
+      <c r="J42" s="15">
+        <f>I42*B42</f>
+        <v>736.95299999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B43" s="10">
         <v>1</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="12">
-        <f>H58</f>
-        <v>4.5</v>
+        <f>H43</f>
+        <v>31</v>
       </c>
       <c r="G43" s="12">
-        <f t="shared" si="14"/>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="20">
-        <f>SUM(G39:G43)</f>
-        <v>384.7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="22">
-        <f>G44*0.16</f>
-        <v>61.552</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="19" t="s">
+        <f t="shared" si="18"/>
+        <v>31</v>
+      </c>
+      <c r="H43" s="13">
+        <v>31</v>
+      </c>
+      <c r="I43" s="14">
+        <f t="shared" si="19"/>
+        <v>618.44999999999993</v>
+      </c>
+      <c r="J43" s="15">
+        <f>I43*B43</f>
+        <v>618.44999999999993</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="23">
+        <v>16</v>
+      </c>
+      <c r="B44" s="35">
+        <v>1</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38">
+        <f>H44</f>
+        <v>587.5</v>
+      </c>
+      <c r="G44" s="38">
+        <f t="shared" si="18"/>
+        <v>587.5</v>
+      </c>
+      <c r="H44" s="13">
+        <v>587.5</v>
+      </c>
+      <c r="I44" s="14">
+        <f t="shared" si="19"/>
+        <v>11720.625</v>
+      </c>
+      <c r="J44" s="15">
+        <f>I44*B44</f>
+        <v>11720.625</v>
+      </c>
+      <c r="K44" s="32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="23">
+        <v>17</v>
+      </c>
+      <c r="B45" s="10">
+        <v>1</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" s="39"/>
+      <c r="F45" s="12">
+        <f>H45</f>
+        <v>0.60150375939849621</v>
+      </c>
+      <c r="G45" s="12">
+        <f t="shared" ref="G45" si="20">F45*B45</f>
+        <v>0.60150375939849621</v>
+      </c>
+      <c r="H45" s="13">
+        <f>I45/I5</f>
+        <v>0.60150375939849621</v>
+      </c>
+      <c r="I45" s="14">
         <v>12</v>
       </c>
-      <c r="G46" s="22">
-        <f>G44+G45</f>
-        <v>446.25200000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F47" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G47" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="J45" s="15">
+        <f>I45*B45</f>
+        <v>12</v>
+      </c>
+      <c r="K45" s="41"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F46" s="29"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="15"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="15"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="15"/>
+      <c r="L48" s="40"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23">
+        <v>18</v>
+      </c>
+      <c r="B50" s="10">
+        <v>1</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="12">
+        <f>H50</f>
+        <v>1823</v>
+      </c>
+      <c r="G50" s="12">
+        <f>F50*B50</f>
+        <v>1823</v>
+      </c>
+      <c r="H50" s="13">
+        <v>1823</v>
+      </c>
+      <c r="I50" s="14">
+        <f>H50*$I$5</f>
+        <v>36368.85</v>
+      </c>
+      <c r="J50" s="15">
+        <f>I50*B50</f>
+        <v>36368.85</v>
+      </c>
+      <c r="K50" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="23">
+        <v>19</v>
+      </c>
+      <c r="B51" s="10">
+        <v>1</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12">
+        <f>H51</f>
+        <v>2192.5</v>
+      </c>
+      <c r="G51" s="12">
+        <f t="shared" ref="G51:G53" si="21">F51*B51</f>
+        <v>2192.5</v>
+      </c>
+      <c r="H51" s="13">
+        <v>2192.5</v>
+      </c>
+      <c r="I51" s="14">
+        <f t="shared" ref="I51:I52" si="22">H51*$I$5</f>
+        <v>43740.375</v>
+      </c>
+      <c r="J51" s="15">
+        <f>I51*B51</f>
+        <v>43740.375</v>
+      </c>
+      <c r="K51" s="43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23">
         <v>20</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
-        <v>13</v>
       </c>
       <c r="B52" s="10">
         <v>1</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="12">
-        <f>H71</f>
-        <v>75</v>
+        <f>H52</f>
+        <v>825.75</v>
       </c>
       <c r="G52" s="12">
-        <f>F52*B52</f>
-        <v>75</v>
-      </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-    </row>
-    <row r="53" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="21"/>
+        <v>825.75</v>
+      </c>
+      <c r="H52" s="13">
+        <v>825.75</v>
+      </c>
+      <c r="I52" s="14">
+        <f t="shared" si="22"/>
+        <v>16473.712499999998</v>
+      </c>
+      <c r="J52" s="15">
+        <f>I52*B52</f>
+        <v>16473.712499999998</v>
+      </c>
+      <c r="K52" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B53" s="10">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="E53" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="16"/>
       <c r="F53" s="12">
-        <f>H72</f>
-        <v>36.94</v>
+        <f>H53</f>
+        <v>10.025062656641605</v>
       </c>
       <c r="G53" s="12">
-        <f t="shared" ref="G53:G55" si="15">F53*B53</f>
-        <v>36.94</v>
-      </c>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-    </row>
-    <row r="54" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23">
+        <f t="shared" si="21"/>
+        <v>130.32581453634086</v>
+      </c>
+      <c r="H53" s="13">
+        <f>I53/I5</f>
+        <v>10.025062656641605</v>
+      </c>
+      <c r="I53" s="14">
+        <v>200</v>
+      </c>
+      <c r="J53" s="15">
+        <f>I53*B53</f>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" s="20">
+        <f>SUM(G13:G53)</f>
+        <v>9685.9273182957404</v>
+      </c>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="15">
+        <f>SUM(J13:J53)</f>
+        <v>193234.24999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="17"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="22">
+        <f>G54*0.16</f>
+        <v>1549.7483709273185</v>
+      </c>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="15"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="22">
+        <f>G54+G55</f>
+        <v>11235.675689223059</v>
+      </c>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="15">
+        <f>J54*1.16</f>
+        <v>224151.72999999995</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F57" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="10">
-        <v>1</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="12">
-        <f>H73</f>
-        <v>31</v>
-      </c>
-      <c r="G54" s="12">
-        <f t="shared" si="15"/>
-        <v>31</v>
-      </c>
-      <c r="H54" s="13">
-        <v>229</v>
-      </c>
-      <c r="I54" s="14">
-        <f>H54*$I$5</f>
-        <v>4568.55</v>
-      </c>
-      <c r="J54" s="15">
-        <f>I54*B39</f>
-        <v>4568.55</v>
-      </c>
-      <c r="K54" s="31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="23">
+      <c r="G57" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B55" s="35">
-        <v>1</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="37"/>
-      <c r="F55" s="38">
-        <f>H74</f>
-        <v>587.5</v>
-      </c>
-      <c r="G55" s="38">
-        <f t="shared" si="15"/>
-        <v>587.5</v>
-      </c>
-      <c r="H55" s="13">
-        <v>4.75</v>
-      </c>
-      <c r="I55" s="14">
-        <f t="shared" ref="I55:I57" si="16">H55*$I$5</f>
-        <v>94.762500000000003</v>
-      </c>
-      <c r="J55" s="15">
-        <f>I55*B40</f>
-        <v>94.762500000000003</v>
-      </c>
-      <c r="K55" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23">
-        <v>17</v>
-      </c>
-      <c r="B56" s="10">
-        <v>1</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D56" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" s="41"/>
-      <c r="F56" s="12">
-        <f>H75</f>
-        <v>0.60150375939849621</v>
-      </c>
-      <c r="G56" s="12">
-        <f t="shared" ref="G56" si="17">F56*B56</f>
-        <v>0.60150375939849621</v>
-      </c>
-      <c r="H56" s="13">
-        <v>5.2</v>
-      </c>
-      <c r="I56" s="14">
-        <f t="shared" si="16"/>
-        <v>103.74</v>
-      </c>
-      <c r="J56" s="15">
-        <f>I56*B41</f>
-        <v>103.74</v>
-      </c>
-      <c r="K56" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="40">
-        <f>SUM(G52:G55)</f>
-        <v>730.44</v>
-      </c>
-      <c r="H57" s="13">
-        <v>141.25</v>
-      </c>
-      <c r="I57" s="14">
-        <f t="shared" si="16"/>
-        <v>2817.9375</v>
-      </c>
-      <c r="J57" s="15">
-        <f>I57*B42</f>
-        <v>2817.9375</v>
-      </c>
-      <c r="K57" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="22">
-        <f>G57*0.16</f>
-        <v>116.87040000000002</v>
-      </c>
-      <c r="H58" s="13">
-        <v>4.5</v>
-      </c>
-      <c r="I58" s="14">
-        <f>H58*$I$5</f>
-        <v>89.774999999999991</v>
-      </c>
-      <c r="J58" s="15">
-        <f>I58*B43</f>
-        <v>89.774999999999991</v>
-      </c>
-      <c r="K58" s="32" t="s">
-        <v>44</v>
+      <c r="A58" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="22">
-        <f>G57+G58</f>
-        <v>847.31040000000007</v>
-      </c>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="15">
-        <f>SUM(J54:J58)</f>
-        <v>7674.7649999999994</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F60" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G60" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H60" s="21"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="15"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F61" s="29"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="15">
-        <f>J59*1.16</f>
-        <v>8902.7273999999979</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F62" s="29"/>
-      <c r="G62" s="30"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F63" s="29"/>
-      <c r="G63" s="30"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F64" s="29"/>
-      <c r="G64" s="30"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F65" s="29"/>
-      <c r="G65" s="30"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F66" s="29"/>
-      <c r="G66" s="30"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F67" s="29"/>
-      <c r="G67" s="30"/>
-    </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="23">
-        <v>18</v>
-      </c>
-      <c r="B71" s="10">
-        <v>1</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="F71" s="12">
-        <f>H92</f>
-        <v>1823</v>
-      </c>
-      <c r="G71" s="12">
-        <f>F71*B71</f>
-        <v>1823</v>
-      </c>
-      <c r="H71" s="13">
-        <v>75</v>
-      </c>
-      <c r="I71" s="14">
-        <f>H71*$I$5</f>
-        <v>1496.25</v>
-      </c>
-      <c r="J71" s="15">
-        <f>I71*B52</f>
-        <v>1496.25</v>
-      </c>
-      <c r="K71" s="32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="23">
-        <v>19</v>
-      </c>
-      <c r="B72" s="10">
-        <v>1</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="E72" s="11"/>
-      <c r="F72" s="12">
-        <f>H93</f>
-        <v>2192.5</v>
-      </c>
-      <c r="G72" s="12">
-        <f t="shared" ref="G72:G74" si="18">F72*B72</f>
-        <v>2192.5</v>
-      </c>
-      <c r="H72" s="13">
-        <v>36.94</v>
-      </c>
-      <c r="I72" s="14">
-        <f t="shared" ref="I72:I74" si="19">H72*$I$5</f>
-        <v>736.95299999999997</v>
-      </c>
-      <c r="J72" s="15">
-        <f>I72*B53</f>
-        <v>736.95299999999997</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23">
-        <v>20</v>
-      </c>
-      <c r="B73" s="10">
-        <v>1</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E73" s="11"/>
-      <c r="F73" s="12">
-        <f>H94</f>
-        <v>825.75</v>
-      </c>
-      <c r="G73" s="12">
-        <f t="shared" si="18"/>
-        <v>825.75</v>
-      </c>
-      <c r="H73" s="13">
-        <v>31</v>
-      </c>
-      <c r="I73" s="14">
-        <f t="shared" si="19"/>
-        <v>618.44999999999993</v>
-      </c>
-      <c r="J73" s="15">
-        <f>I73*B54</f>
-        <v>618.44999999999993</v>
-      </c>
-      <c r="K73" s="32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="23">
-        <v>21</v>
-      </c>
-      <c r="B74" s="10">
-        <v>1</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="E74" s="16"/>
-      <c r="F74" s="12">
-        <f>H95</f>
-        <v>10.025062656641605</v>
-      </c>
-      <c r="G74" s="12">
-        <f t="shared" si="18"/>
-        <v>10.025062656641605</v>
-      </c>
-      <c r="H74" s="13">
-        <v>587.5</v>
-      </c>
-      <c r="I74" s="14">
-        <f t="shared" si="19"/>
-        <v>11720.625</v>
-      </c>
-      <c r="J74" s="15">
-        <f>I74*B55</f>
-        <v>11720.625</v>
-      </c>
-      <c r="K74" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="L74"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G75" s="20">
-        <f>SUM(G71:G74)</f>
-        <v>4851.2750626566412</v>
-      </c>
-      <c r="H75" s="13">
-        <f>I75/I5</f>
-        <v>0.60150375939849621</v>
-      </c>
-      <c r="I75" s="14">
-        <v>12</v>
-      </c>
-      <c r="J75" s="15">
-        <f>I75*B56</f>
-        <v>12</v>
-      </c>
-      <c r="K75" s="43"/>
-      <c r="L75" s="42"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" s="22">
-        <f>G75*0.16</f>
-        <v>776.20401002506264</v>
-      </c>
-      <c r="H76" s="21"/>
-      <c r="I76" s="21"/>
-      <c r="J76" s="15">
-        <f>SUM(J71:J74)</f>
-        <v>14572.278</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="18"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G77" s="22">
-        <f>G75+G76</f>
-        <v>5627.4790726817037</v>
-      </c>
-      <c r="H77" s="21"/>
-      <c r="I77" s="21"/>
-      <c r="J77" s="15"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F78" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H78" s="21"/>
-      <c r="I78" s="21"/>
-      <c r="J78" s="15">
-        <f>J76*1.16</f>
-        <v>16903.842479999999</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F80" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G80" s="22">
-        <f>G20+G33+G46+G59+G77</f>
-        <v>11095.429072681705</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>41</v>
-      </c>
-      <c r="I81" s="44">
-        <f>G80*I5</f>
-        <v>221353.81000000003</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H92" s="13">
-        <v>1823</v>
-      </c>
-      <c r="I92" s="14">
-        <f>H92*$I$5</f>
-        <v>36368.85</v>
-      </c>
-      <c r="J92" s="15">
-        <f>I92*B71</f>
-        <v>36368.85</v>
-      </c>
-      <c r="K92" s="32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H93" s="13">
-        <v>2192.5</v>
-      </c>
-      <c r="I93" s="14">
-        <f t="shared" ref="I93:I94" si="20">H93*$I$5</f>
-        <v>43740.375</v>
-      </c>
-      <c r="J93" s="15">
-        <f>I93*B72</f>
-        <v>43740.375</v>
-      </c>
-      <c r="K93" s="45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H94" s="13">
-        <v>825.75</v>
-      </c>
-      <c r="I94" s="14">
-        <f t="shared" si="20"/>
-        <v>16473.712499999998</v>
-      </c>
-      <c r="J94" s="15">
-        <f>I94*B73</f>
-        <v>16473.712499999998</v>
-      </c>
-      <c r="K94" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H95" s="13">
-        <f>I95/I5</f>
-        <v>10.025062656641605</v>
-      </c>
-      <c r="I95" s="14">
-        <v>200</v>
-      </c>
-      <c r="J95" s="15">
-        <f>I95*B74</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H96" s="21"/>
-      <c r="I96" s="21"/>
-      <c r="J96" s="15">
-        <f>SUM(J92:J95)</f>
-        <v>96782.9375</v>
-      </c>
-    </row>
-    <row r="97" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H97" s="21"/>
-      <c r="I97" s="21"/>
-      <c r="J97" s="15"/>
-    </row>
-    <row r="98" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H98" s="21"/>
-      <c r="I98" s="21"/>
-      <c r="J98" s="15">
-        <f>J96*1.16</f>
-        <v>112268.20749999999</v>
-      </c>
-    </row>
-    <row r="101" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="J101" s="44">
-        <f>G80*I5</f>
-        <v>221353.81000000003</v>
-      </c>
+      <c r="J59" s="42"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.43" right="0.31" top="0.66" bottom="0.89" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="78" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.43307086614173229" right="0.31496062992125984" top="0.6692913385826772" bottom="0.9055118110236221" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="5" scale="74" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>